<commit_message>
input prep (corr. c2c)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/for paper/input c2c.xlsx
+++ b/migforecasting/clustering/for paper/input c2c.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,16 +1231,16 @@
         <v>1278.9999999999998</v>
       </c>
       <c r="C17" s="1">
+        <v>19406.97712</v>
+      </c>
+      <c r="D17" s="1">
         <v>2585.4999999999986</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>281.99999999999972</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>415783.74875999975</v>
-      </c>
-      <c r="F17" s="1">
-        <v>46.954686477696221</v>
       </c>
       <c r="G17" s="1">
         <v>37.299999999999997</v>
@@ -1281,16 +1281,16 @@
         <v>2086.9999999999986</v>
       </c>
       <c r="C18" s="1">
+        <v>17100.190320000002</v>
+      </c>
+      <c r="D18" s="1">
         <v>6433.2999999999956</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>210.99999999999983</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>267414.72803999996</v>
-      </c>
-      <c r="F18" s="1">
-        <v>14.994657846809471</v>
       </c>
       <c r="G18" s="1">
         <v>32.08</v>
@@ -1331,16 +1331,16 @@
         <v>2688.9999999999995</v>
       </c>
       <c r="C19" s="1">
+        <v>18039.2</v>
+      </c>
+      <c r="D19" s="1">
         <v>9015.3999999999905</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>204.99999999999977</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>229243.99999999988</v>
-      </c>
-      <c r="F19" s="1">
-        <v>10.305880237367379</v>
       </c>
       <c r="G19" s="1">
         <v>21.93</v>
@@ -1381,16 +1381,16 @@
         <v>4696.9999999999991</v>
       </c>
       <c r="C20" s="1">
+        <v>19598.053680000001</v>
+      </c>
+      <c r="D20" s="1">
         <v>27639.699999999986</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>219.99999999999972</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>794230.03655999957</v>
-      </c>
-      <c r="F20" s="1">
-        <v>22.599949821016981</v>
       </c>
       <c r="G20" s="1">
         <v>22.85</v>
@@ -1431,16 +1431,16 @@
         <v>5471</v>
       </c>
       <c r="C21" s="1">
+        <v>24531.17148999999</v>
+      </c>
+      <c r="D21" s="1">
         <v>9993.7999999999938</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>349.99999999999949</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>135007.86686999991</v>
-      </c>
-      <c r="F21" s="1">
-        <v>4.2340797487925723</v>
       </c>
       <c r="G21" s="1">
         <v>22.88</v>

</xml_diff>